<commit_message>
Everything working. Push manually.
</commit_message>
<xml_diff>
--- a/book.xlsx
+++ b/book.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasonkuruzovich/GitHub/ms-website-fall-2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1D0D5E7-F6D3-164C-A1AD-2D6CBAFF8E06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97BDEF6D-9C56-7148-8E60-629EF070C8EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INTROML" sheetId="25" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="167">
   <si>
     <t>Day</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Topic</t>
   </si>
   <si>
-    <t>Reading</t>
-  </si>
-  <si>
     <t>Link</t>
   </si>
   <si>
@@ -339,9 +336,6 @@
     <t>Basic Data Structures</t>
   </si>
   <si>
-    <t>File name</t>
-  </si>
-  <si>
     <t>textbook_logo</t>
   </si>
   <si>
@@ -541,6 +535,9 @@
   </si>
   <si>
     <t>assignments/02starter</t>
+  </si>
+  <si>
+    <t>IMS Chapter 2</t>
   </si>
 </sst>
 </file>
@@ -1111,10 +1108,10 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="11" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C4" s="29" t="s">
         <v>1</v>
@@ -1145,10 +1142,10 @@
         <v>Mon</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1166,10 +1163,10 @@
         <v>Thu</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="11" customFormat="1">
@@ -1184,10 +1181,10 @@
         <v>Mon</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1205,10 +1202,10 @@
         <v>Tue</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1227,10 +1224,10 @@
         <v>Thu</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1249,10 +1246,10 @@
         <v>Mon</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -1271,10 +1268,10 @@
         <v>Thu</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -1293,10 +1290,10 @@
         <v>Mon</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -1315,10 +1312,10 @@
         <v>Thu</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1337,10 +1334,10 @@
         <v>Mon</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1359,10 +1356,10 @@
         <v>Thu</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1381,10 +1378,10 @@
         <v>Mon</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1403,10 +1400,10 @@
         <v>Thu</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1421,10 +1418,10 @@
         <v>Mon</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1442,10 +1439,10 @@
         <v>Thu</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1464,10 +1461,10 @@
         <v>Mon</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1486,10 +1483,10 @@
         <v>Thu</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1508,10 +1505,10 @@
         <v>Mon</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1530,10 +1527,10 @@
         <v>Thu</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1552,10 +1549,10 @@
         <v>Mon</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1574,10 +1571,10 @@
         <v>Thu</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F25" s="11" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1596,10 +1593,10 @@
         <v>Mon</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1618,10 +1615,10 @@
         <v>Thu</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F27" s="11" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1640,10 +1637,10 @@
         <v>Mon</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F28" s="11" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1662,10 +1659,10 @@
         <v>Thu</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F29" s="11" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1680,10 +1677,10 @@
         <v>Mon</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1701,10 +1698,10 @@
         <v>Thu</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F31" s="11" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1722,10 +1719,10 @@
         <v>Mon</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F32" s="11" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1744,10 +1741,10 @@
         <v>Thu</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1766,10 +1763,10 @@
         <v>Mon</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F34" s="11" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1788,23 +1785,23 @@
         <v>Thu</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F35" s="11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="11"/>
       <c r="C36" s="30" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D36" s="30"/>
       <c r="E36" s="11" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F36" s="11" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G36" s="11"/>
     </row>
@@ -2087,17 +2084,17 @@
   <sheetData>
     <row r="4" spans="1:3">
       <c r="A4" s="6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="B5" s="11" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="B6" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2117,15 +2114,15 @@
     </row>
     <row r="10" spans="1:3">
       <c r="B10" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="19">
       <c r="B11" s="31" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -2137,12 +2134,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:V955"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B23" sqref="B23"/>
       <selection pane="topRight" activeCell="B23" sqref="B23"/>
       <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
@@ -2159,10 +2156,10 @@
   <sheetData>
     <row r="1" spans="1:22" s="12" customFormat="1" ht="19">
       <c r="A1" s="11" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C1" s="29" t="s">
         <v>1</v>
@@ -2174,10 +2171,10 @@
         <v>2</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G1" s="31" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H1" s="31"/>
     </row>
@@ -2196,10 +2193,10 @@
         <v>Mon</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G2" s="11">
         <v>1</v>
@@ -2220,10 +2217,10 @@
         <v>Thu</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G3" s="11">
         <v>1</v>
@@ -2242,11 +2239,11 @@
         <v>Mon</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F4" s="11"/>
       <c r="G4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:22">
@@ -2264,10 +2261,10 @@
         <v>Tue</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G5" s="5">
         <v>1</v>
@@ -2289,10 +2286,10 @@
         <v>Thu</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G6" s="5">
         <v>1</v>
@@ -2314,10 +2311,10 @@
         <v>Mon</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G7" s="5">
         <v>0</v>
@@ -2339,10 +2336,10 @@
         <v>Thu</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G8" s="5">
         <v>0</v>
@@ -2364,10 +2361,10 @@
         <v>Mon</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G9" s="5">
         <v>0</v>
@@ -2389,10 +2386,10 @@
         <v>Thu</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G10" s="5">
         <v>0</v>
@@ -2429,10 +2426,10 @@
         <v>Mon</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G11" s="5">
         <v>0</v>
@@ -2469,10 +2466,10 @@
         <v>Thu</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G12" s="5">
         <v>0</v>
@@ -2509,10 +2506,10 @@
         <v>Mon</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G13" s="5">
         <v>0</v>
@@ -2549,10 +2546,10 @@
         <v>Thu</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G14" s="5">
         <v>0</v>
@@ -2586,10 +2583,10 @@
         <v>Mon</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G15" s="5">
         <v>0</v>
@@ -2625,10 +2622,10 @@
         <v>Thu</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G16" s="5">
         <v>0</v>
@@ -2665,10 +2662,10 @@
         <v>Mon</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G17" s="5">
         <v>0</v>
@@ -2705,10 +2702,10 @@
         <v>Thu</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G18" s="5">
         <v>0</v>
@@ -2745,10 +2742,10 @@
         <v>Mon</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G19" s="5">
         <v>0</v>
@@ -2785,10 +2782,10 @@
         <v>Thu</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G20" s="5">
         <v>0</v>
@@ -2825,10 +2822,10 @@
         <v>Mon</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G21" s="5">
         <v>0</v>
@@ -2865,10 +2862,10 @@
         <v>Thu</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G22" s="5">
         <v>0</v>
@@ -2905,10 +2902,10 @@
         <v>Mon</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G23" s="5">
         <v>0</v>
@@ -2945,10 +2942,10 @@
         <v>Thu</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G24" s="5">
         <v>0</v>
@@ -2985,10 +2982,10 @@
         <v>Mon</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G25" s="5">
         <v>0</v>
@@ -3025,10 +3022,10 @@
         <v>Thu</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G26" s="5">
         <v>0</v>
@@ -3062,10 +3059,10 @@
         <v>Mon</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G27" s="5">
         <v>0</v>
@@ -3101,10 +3098,10 @@
         <v>Thu</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G28" s="5">
         <v>0</v>
@@ -3140,10 +3137,10 @@
         <v>Mon</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G29" s="5">
         <v>0</v>
@@ -3180,10 +3177,10 @@
         <v>Thu</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G30" s="5">
         <v>0</v>
@@ -3220,10 +3217,10 @@
         <v>Mon</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G31" s="5">
         <v>0</v>
@@ -3260,10 +3257,10 @@
         <v>Thu</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G32" s="5">
         <v>0</v>
@@ -3294,10 +3291,10 @@
       <c r="C33" s="30"/>
       <c r="D33" s="30"/>
       <c r="E33" s="11" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G33" s="5">
         <v>0</v>
@@ -7945,7 +7942,7 @@
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B23" sqref="B23"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -7959,16 +7956,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="12" customFormat="1" ht="19">
       <c r="A1" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>3</v>
+        <v>148</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17">
@@ -7976,15 +7973,20 @@
         <v>2</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C2" s="10"/>
       <c r="D2" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="B3" s="8"/>
+        <v>156</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="17">
+      <c r="A3" s="14">
+        <v>3</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>166</v>
+      </c>
       <c r="C3" s="10"/>
     </row>
     <row r="4" spans="1:4">
@@ -8100,7 +8102,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -8112,16 +8114,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="12" customFormat="1" ht="19">
       <c r="A1" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>100</v>
+        <v>155</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17">
@@ -8129,13 +8131,13 @@
         <v>2</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17">
@@ -8143,13 +8145,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17">
@@ -8157,13 +8159,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C4" s="35" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -8439,7 +8441,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{929EBF5B-C504-F94A-BB00-B01380980449}">
   <dimension ref="A1:E922"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -8455,19 +8457,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="12" customFormat="1" ht="19">
       <c r="A1" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B1" s="32" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D1" s="31" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E1" s="31" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="68" customHeight="1">
@@ -8475,16 +8477,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D2" s="30">
         <v>44081</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="17">
@@ -8492,16 +8494,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="33" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D3" s="29">
         <v>44084</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -11285,7 +11287,7 @@
         <v>43703</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1">
@@ -11293,7 +11295,7 @@
         <v>43705</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" customHeight="1">
@@ -11301,7 +11303,7 @@
         <v>43706</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" customHeight="1">
@@ -11309,7 +11311,7 @@
         <v>43707</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" customHeight="1">
@@ -11323,7 +11325,7 @@
         <v>43710</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.75" customHeight="1">
@@ -11331,7 +11333,7 @@
         <v>43711</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" customHeight="1">
@@ -11339,7 +11341,7 @@
         <v>43721</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15.75" customHeight="1">
@@ -11347,15 +11349,15 @@
         <v>43728</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.75" customHeight="1">
       <c r="A10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.75" customHeight="1">
@@ -11369,7 +11371,7 @@
         <v>43752</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15.75" customHeight="1">
@@ -11377,15 +11379,15 @@
         <v>43753</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15.75" customHeight="1">
       <c r="A14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15.75" customHeight="1">
@@ -11393,15 +11395,15 @@
         <v>43757</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="15.75" customHeight="1">
       <c r="A16" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15.75" customHeight="1">
@@ -11409,7 +11411,7 @@
         <v>43763</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15.75" customHeight="1">
@@ -11420,10 +11422,10 @@
     </row>
     <row r="19" spans="1:2" ht="15.75" customHeight="1">
       <c r="A19" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15.75" customHeight="1">
@@ -11431,15 +11433,15 @@
         <v>43770</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="15.75" customHeight="1">
       <c r="A21" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15.75" customHeight="1">
@@ -11447,7 +11449,7 @@
         <v>43777</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15.75" customHeight="1">
@@ -11455,7 +11457,7 @@
         <v>43787</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="15.75" customHeight="1">
@@ -11463,7 +11465,7 @@
         <v>43791</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="15.75" customHeight="1">
@@ -11471,15 +11473,15 @@
         <v>43795</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15.75" customHeight="1">
       <c r="A26" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15.75" customHeight="1">
@@ -11493,7 +11495,7 @@
         <v>43800</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15.75" customHeight="1">
@@ -11501,7 +11503,7 @@
         <v>43801</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15.75" customHeight="1">
@@ -11509,7 +11511,7 @@
         <v>43801</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15.75" customHeight="1">
@@ -11517,15 +11519,15 @@
         <v>43810</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15.75" customHeight="1">
       <c r="A32" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15.75" customHeight="1">
@@ -11533,15 +11535,15 @@
         <v>43815</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15.75" customHeight="1">
       <c r="A34" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="15.75" customHeight="1">
@@ -11549,15 +11551,15 @@
         <v>43820</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15.75" customHeight="1">
       <c r="A36" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15.75" customHeight="1">
@@ -11565,7 +11567,7 @@
         <v>43830</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="15.75" customHeight="1">
@@ -11576,10 +11578,10 @@
     </row>
     <row r="39" spans="1:2" ht="15.75" customHeight="1">
       <c r="A39" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="15.75" customHeight="1">
@@ -11587,7 +11589,7 @@
         <v>43833</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="15.75" customHeight="1">
@@ -11595,7 +11597,7 @@
         <v>43842</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="15.75" customHeight="1">
@@ -11603,7 +11605,7 @@
         <v>43843</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="15.75" customHeight="1">
@@ -11611,7 +11613,7 @@
         <v>43850</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="15.75" customHeight="1">
@@ -11619,7 +11621,7 @@
         <v>43854</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="15.75" customHeight="1">
@@ -11633,7 +11635,7 @@
         <v>43868</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="15.75" customHeight="1">
@@ -11641,7 +11643,7 @@
         <v>43878</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="15.75" customHeight="1">
@@ -11649,7 +11651,7 @@
         <v>43879</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="15.75" customHeight="1">
@@ -11663,15 +11665,15 @@
         <v>43892</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="15.75" customHeight="1">
       <c r="A51" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B51" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="15.75" customHeight="1">
@@ -11679,15 +11681,15 @@
         <v>43896</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="15.75" customHeight="1">
       <c r="A53" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B53" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="15.75" customHeight="1">
@@ -11695,7 +11697,7 @@
         <v>43905</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="15.75" customHeight="1">
@@ -11703,15 +11705,15 @@
         <v>43906</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="15.75" customHeight="1">
       <c r="A56" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B56" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="15.75" customHeight="1">
@@ -11719,7 +11721,7 @@
         <v>43915</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="15.75" customHeight="1">
@@ -11727,7 +11729,7 @@
         <v>43917</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="15.75" customHeight="1">
@@ -11741,7 +11743,7 @@
         <v>43931</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="15.75" customHeight="1">
@@ -11749,7 +11751,7 @@
         <v>43945</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="15.75" customHeight="1">
@@ -11757,15 +11759,15 @@
         <v>43950</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="15.75" customHeight="1">
       <c r="A63" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="15.75" customHeight="1">
@@ -11773,7 +11775,7 @@
         <v>43951</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="15.75" customHeight="1">
@@ -11784,10 +11786,10 @@
     </row>
     <row r="66" spans="1:2" ht="15.75" customHeight="1">
       <c r="A66" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="15.75" customHeight="1">
@@ -11795,15 +11797,15 @@
         <v>43955</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="15.75" customHeight="1">
       <c r="A68" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B68" s="3" t="s">
         <v>72</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="15.75" customHeight="1">
@@ -11811,7 +11813,7 @@
         <v>43955</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="15.75" customHeight="1">
@@ -11819,7 +11821,7 @@
         <v>43959</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="15.75" customHeight="1">
@@ -11827,7 +11829,7 @@
         <v>43960</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="15.75" customHeight="1">
@@ -11835,7 +11837,7 @@
         <v>43973</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="15.75" customHeight="1">
@@ -11843,7 +11845,7 @@
         <v>43974</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="15.75" customHeight="1">
@@ -11851,7 +11853,7 @@
         <v>43974</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="15.75" customHeight="1"/>
@@ -12879,7 +12881,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B1" s="9" t="e">
         <f>#REF!</f>
@@ -12888,7 +12890,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B2" s="7" t="e">
         <f>#REF!</f>
@@ -12897,7 +12899,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B3" s="7" t="e">
         <f>#REF!</f>
@@ -12906,7 +12908,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B4" s="7" t="e">
         <f>#REF!</f>
@@ -12915,7 +12917,7 @@
     </row>
     <row r="5" spans="1:2" s="1" customFormat="1">
       <c r="A5" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B5" s="24" t="e">
         <f>IF(ISBLANK(#REF!),"",#REF!)</f>
@@ -12924,7 +12926,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B6" s="9" t="e">
         <f>#REF!</f>
@@ -12933,7 +12935,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="25" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B7" s="7" t="e">
         <f>#REF!</f>
@@ -12942,7 +12944,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="25" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B8" s="7" t="e">
         <f>#REF!</f>

</xml_diff>